<commit_message>
Rename folders MvvmFx.Windows to MvvmFx.Bindings (#184)
</commit_message>
<xml_diff>
--- a/Documentation/MvvmFx name organizer.xlsx
+++ b/Documentation/MvvmFx name organizer.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>MvvmFx-WinForms</t>
   </si>
@@ -40,9 +40,6 @@
     <t>NuGet id</t>
   </si>
   <si>
-    <t>MvvmFx.Windows.WinForms</t>
-  </si>
-  <si>
     <t>WindowsBase.WinForms</t>
   </si>
   <si>
@@ -52,30 +49,9 @@
     <t>WindowsBase.WisejWeb</t>
   </si>
   <si>
-    <t>MvvmFx.Windows.WPF</t>
-  </si>
-  <si>
-    <t>MvvmFx.Windows.WisejWeb</t>
-  </si>
-  <si>
-    <t>MvvmFx.Windows</t>
-  </si>
-  <si>
-    <t>Binding\MvvmFx.Windows</t>
-  </si>
-  <si>
     <t>MvvmFx.DataBinding.WisejWeb</t>
   </si>
   <si>
-    <t>MvvmFx-WPF</t>
-  </si>
-  <si>
-    <t>MvvmFx-Wisej</t>
-  </si>
-  <si>
-    <t>MvvmFx-Desktop</t>
-  </si>
-  <si>
     <t>Desktop</t>
   </si>
   <si>
@@ -88,18 +64,9 @@
     <t>WPF</t>
   </si>
   <si>
-    <t>Binding\MvvmFx.Windows.WinForms</t>
-  </si>
-  <si>
     <t>Binding\WindowsBase.WinForms</t>
   </si>
   <si>
-    <t>Binding\MvvmFx.Windows.WPF</t>
-  </si>
-  <si>
-    <t>Binding\MvvmFx.Windows.WisejWeb</t>
-  </si>
-  <si>
     <t>Binding\WindowsBase.WisejWeb</t>
   </si>
   <si>
@@ -200,6 +167,48 @@
   </si>
   <si>
     <t>MvvmFx-CaliburnMicro-Csla-WinForms</t>
+  </si>
+  <si>
+    <t>(note)</t>
+  </si>
+  <si>
+    <t>Package name changed for clarity and consistencey</t>
+  </si>
+  <si>
+    <t>MvvmFx.Bindings.WPF</t>
+  </si>
+  <si>
+    <t>Binding\MvvmFx.Bindings.WPF</t>
+  </si>
+  <si>
+    <t>MvvmFx.Bindings.WinForms</t>
+  </si>
+  <si>
+    <t>Binding\MvvmFx.Bindings.WinForms</t>
+  </si>
+  <si>
+    <t>MvvmFx.Bindings.WisejWeb</t>
+  </si>
+  <si>
+    <t>Binding\MvvmFx.Bindings.WisejWeb</t>
+  </si>
+  <si>
+    <t>MvvmFx.Bindings</t>
+  </si>
+  <si>
+    <t>Binding\MvvmFx.Bindings</t>
+  </si>
+  <si>
+    <t>MvvmFx-Bindings-Desktop</t>
+  </si>
+  <si>
+    <t>MvvmFx-Bindings-WPF</t>
+  </si>
+  <si>
+    <t>MvvmFx-Bindings-WinForms</t>
+  </si>
+  <si>
+    <t>MvvmFx-Bindings-Wisej</t>
   </si>
 </sst>
 </file>
@@ -374,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -401,9 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -419,6 +425,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,11 +732,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,18 +754,18 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="22"/>
+        <v>24</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -785,415 +797,430 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="38"/>
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="34"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="15"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="29" t="s">
+      <c r="C25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="D25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="17"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
-      <c r="B27" s="34" t="s">
-        <v>21</v>
+      <c r="B27" s="33" t="s">
+        <v>13</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="A28" s="10"/>
+      <c r="B28" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="9"/>
+      <c r="D28" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="15" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="15"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="20" t="s">
+      <c r="E32" s="15"/>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="17"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="17"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>